<commit_message>
Working with splitting the events table
</commit_message>
<xml_diff>
--- a/output_data/101_midi_1.xlsx
+++ b/output_data/101_midi_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\MSc-neuroscience\auditory-experiment-code\output_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33FDE516-D553-4A6B-A71C-664A8D8B7932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A88BC34-6100-41B2-9834-9C88F4FE96F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11505" xr2:uid="{E544606B-A7BD-4B1E-9EF1-7766CE2ED88D}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11505" xr2:uid="{C1A00304-8E9F-449D-822E-BC9E815E61C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -395,7 +395,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B47715-EAA3-4AD2-AF3D-78C5F9E5AC1D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5970A142-2C20-47CF-A427-0F0E6D9A81C7}">
   <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -407,7 +407,7 @@
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -438,10 +438,10 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>4.4079364999999999</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -461,7 +461,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -478,16 +478,16 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>4.6697771000000001</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>4.6697771000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -501,7 +501,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -518,16 +518,16 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>4.9750078000000002</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
-        <v>4.9750078000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -541,7 +541,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -558,16 +558,16 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>5.3119869</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>5.3119869</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -581,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -598,16 +598,16 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>5.5798945</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>5.5798945</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -621,7 +621,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -638,16 +638,16 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>6.2499829</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12">
-        <v>6.2499829</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -678,16 +678,16 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>6.4874957000000002</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14">
-        <v>6.4874957000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -718,16 +718,16 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>6.7452085000000004</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16">
-        <v>6.7452085000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -741,7 +741,7 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -758,16 +758,16 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>7.0501161000000003</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18">
-        <v>7.0501161000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -781,7 +781,7 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -798,16 +798,16 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>7.3000271999999997</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20">
-        <v>7.3000271999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -838,10 +838,10 @@
         <v>2</v>
       </c>
       <c r="C22">
-        <v>17.280733399999999</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -861,7 +861,7 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -878,16 +878,16 @@
         <v>2</v>
       </c>
       <c r="C24">
-        <v>17.6781246</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24">
-        <v>17.6781246</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -901,7 +901,7 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -918,16 +918,16 @@
         <v>2</v>
       </c>
       <c r="C26">
-        <v>18.061561699999999</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26">
-        <v>18.061561699999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -941,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -958,16 +958,16 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>18.4394098</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28">
-        <v>18.4394098</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -998,16 +998,16 @@
         <v>2</v>
       </c>
       <c r="C30">
-        <v>19.174730499999999</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="F30">
-        <v>19.174730499999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1021,7 +1021,7 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1038,16 +1038,16 @@
         <v>2</v>
       </c>
       <c r="C32">
-        <v>19.673040400000001</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="F32">
-        <v>19.673040400000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1061,7 +1061,7 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1078,16 +1078,16 @@
         <v>2</v>
       </c>
       <c r="C34">
-        <v>20.044680700000001</v>
+        <v>0</v>
       </c>
       <c r="D34">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34">
-        <v>20.044680700000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1101,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1118,16 +1118,16 @@
         <v>2</v>
       </c>
       <c r="C36">
-        <v>20.4615939</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
       <c r="F36">
-        <v>20.4615939</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1141,7 +1141,7 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1158,16 +1158,16 @@
         <v>2</v>
       </c>
       <c r="C38">
-        <v>20.8710667</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38">
-        <v>20.8710667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1181,7 +1181,7 @@
         <v>0</v>
       </c>
       <c r="D39">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1198,16 +1198,16 @@
         <v>2</v>
       </c>
       <c r="C40">
-        <v>21.52017</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
       <c r="F40">
-        <v>21.52017</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1221,7 +1221,7 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1238,10 +1238,10 @@
         <v>3</v>
       </c>
       <c r="C42">
-        <v>26.610530300000001</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -1261,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="D43">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -1278,16 +1278,16 @@
         <v>3</v>
       </c>
       <c r="C44">
-        <v>27.095736299999999</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44">
-        <v>27.095736299999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1301,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="D45">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1318,16 +1318,16 @@
         <v>3</v>
       </c>
       <c r="C46">
-        <v>27.564706900000001</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
       <c r="F46">
-        <v>27.564706900000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1341,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="D47">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -1358,16 +1358,16 @@
         <v>3</v>
       </c>
       <c r="C48">
-        <v>27.955828199999999</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E48">
         <v>1</v>
       </c>
       <c r="F48">
-        <v>27.955828199999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1381,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="D49">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -1398,16 +1398,16 @@
         <v>3</v>
       </c>
       <c r="C50">
-        <v>28.4420939</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E50">
         <v>1</v>
       </c>
       <c r="F50">
-        <v>28.4420939</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1421,7 +1421,7 @@
         <v>0</v>
       </c>
       <c r="D51">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -1438,16 +1438,16 @@
         <v>3</v>
       </c>
       <c r="C52">
-        <v>28.909738600000001</v>
+        <v>0</v>
       </c>
       <c r="D52">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
       <c r="F52">
-        <v>28.909738600000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1461,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="D53">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -1478,16 +1478,16 @@
         <v>3</v>
       </c>
       <c r="C54">
-        <v>29.222826600000001</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E54">
         <v>1</v>
       </c>
       <c r="F54">
-        <v>29.222826600000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1501,7 +1501,7 @@
         <v>0</v>
       </c>
       <c r="D55">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -1518,16 +1518,16 @@
         <v>3</v>
       </c>
       <c r="C56">
-        <v>29.568711100000002</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="F56">
-        <v>29.568711100000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1541,7 +1541,7 @@
         <v>0</v>
       </c>
       <c r="D57">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -1558,16 +1558,16 @@
         <v>3</v>
       </c>
       <c r="C58">
-        <v>29.8930714</v>
+        <v>0</v>
       </c>
       <c r="D58">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E58">
         <v>1</v>
       </c>
       <c r="F58">
-        <v>29.8930714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1581,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="D59">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -1598,16 +1598,16 @@
         <v>3</v>
       </c>
       <c r="C60">
-        <v>30.393508799999999</v>
+        <v>0</v>
       </c>
       <c r="D60">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E60">
         <v>1</v>
       </c>
       <c r="F60">
-        <v>30.393508799999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1621,7 +1621,7 @@
         <v>0</v>
       </c>
       <c r="D61">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -1638,10 +1638,10 @@
         <v>4</v>
       </c>
       <c r="C62">
-        <v>37.840493299999999</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -1661,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -1678,16 +1678,16 @@
         <v>4</v>
       </c>
       <c r="C64">
-        <v>38.2254687</v>
+        <v>0</v>
       </c>
       <c r="D64">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E64">
         <v>1</v>
       </c>
       <c r="F64">
-        <v>38.2254687</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1701,7 +1701,7 @@
         <v>0</v>
       </c>
       <c r="D65">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -1718,16 +1718,16 @@
         <v>4</v>
       </c>
       <c r="C66">
-        <v>38.614756999999997</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E66">
         <v>1</v>
       </c>
       <c r="F66">
-        <v>38.614756999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1741,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="D67">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -1758,16 +1758,16 @@
         <v>4</v>
       </c>
       <c r="C68">
-        <v>38.984326899999999</v>
+        <v>0</v>
       </c>
       <c r="D68">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E68">
         <v>1</v>
       </c>
       <c r="F68">
-        <v>38.984326899999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1781,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -1798,16 +1798,16 @@
         <v>4</v>
       </c>
       <c r="C70">
-        <v>39.562241100000001</v>
+        <v>0</v>
       </c>
       <c r="D70">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E70">
         <v>1</v>
       </c>
       <c r="F70">
-        <v>39.562241100000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -1821,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -1838,16 +1838,16 @@
         <v>4</v>
       </c>
       <c r="C72">
-        <v>40.091960499999999</v>
+        <v>0</v>
       </c>
       <c r="D72">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="E72">
         <v>1</v>
       </c>
       <c r="F72">
-        <v>40.091960499999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1861,7 +1861,7 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -1878,16 +1878,16 @@
         <v>4</v>
       </c>
       <c r="C74">
-        <v>40.480092900000002</v>
+        <v>0</v>
       </c>
       <c r="D74">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E74">
         <v>1</v>
       </c>
       <c r="F74">
-        <v>40.480092900000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -1901,7 +1901,7 @@
         <v>0</v>
       </c>
       <c r="D75">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -1918,16 +1918,16 @@
         <v>4</v>
       </c>
       <c r="C76">
-        <v>40.8687319</v>
+        <v>0</v>
       </c>
       <c r="D76">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E76">
         <v>1</v>
       </c>
       <c r="F76">
-        <v>40.8687319</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -1941,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="D77">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -1958,16 +1958,16 @@
         <v>4</v>
       </c>
       <c r="C78">
-        <v>41.298455099999998</v>
+        <v>0</v>
       </c>
       <c r="D78">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E78">
         <v>1</v>
       </c>
       <c r="F78">
-        <v>41.298455099999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -1981,7 +1981,7 @@
         <v>0</v>
       </c>
       <c r="D79">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -1998,16 +1998,16 @@
         <v>4</v>
       </c>
       <c r="C80">
-        <v>41.860030100000003</v>
+        <v>0</v>
       </c>
       <c r="D80">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E80">
         <v>1</v>
       </c>
       <c r="F80">
-        <v>41.860030100000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2021,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -2036,7 +2036,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{954C6FDC-C0B0-4780-BAF8-DD55DEA94517}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F80CE33-E72E-4354-B983-267C2D7319B6}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2048,7 +2048,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2E6949-0649-4782-991B-3DB5E005876F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF68D5A-B0B3-4F7B-9B34-26EFF170042B}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>